<commit_message>
Ajout fichier css initial sans modif
</commit_message>
<xml_diff>
--- a/annexe/mot clés.xlsx
+++ b/annexe/mot clés.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utilisateur\Documents\Formation_Dev_WEb_OC\Projet\projet 4\annexe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utilisateur\Documents\Formation_Dev_WEb_OC\Projet\projet_4\annexe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -547,7 +547,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>